<commit_message>
add the seeders and update some function
</commit_message>
<xml_diff>
--- a/server/output/Alexandria International School_Users.xlsx
+++ b/server/output/Alexandria International School_Users.xlsx
@@ -22,19 +22,19 @@
     <t>jane.doe@example.com</t>
   </si>
   <si>
-    <t>(|kftEW4)*|%</t>
+    <t>5pK(+UO&gt;_tvR</t>
   </si>
   <si>
     <t>alex.brown@example.com</t>
   </si>
   <si>
-    <t>(03*ASnVOX9i</t>
+    <t>8FC!;Z)1s$y.</t>
   </si>
   <si>
     <t>ava.wilson@example.com</t>
   </si>
   <si>
-    <t>3CWOC0ofi3+n</t>
+    <t>d{.QR2T2Q.BN</t>
   </si>
 </sst>
 </file>

</xml_diff>